<commit_message>
burndown sheet version 1.1
</commit_message>
<xml_diff>
--- a/Planning and Design/Burndown Sheet.xlsx
+++ b/Planning and Design/Burndown Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\CST-247\Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Desktop\CST247\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FA8104-EEBB-4421-AC87-185AC6D4F088}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C832F4FA-61A4-4F0B-A140-9C1C6DA8D716}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Burn Down Chart" sheetId="1" r:id="rId1"/>
     <sheet name="How To Use" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -133,36 +133,27 @@
     <t>After each Daily Standup each Team Member should review the Burn Down Chart to ensure your Sprint will be delivered on time</t>
   </si>
   <si>
+    <t>Team</t>
+  </si>
+  <si>
     <t>Project Title: Minesweeper
-Release #:1.0
-Sprint #: 1</t>
-  </si>
-  <si>
-    <t>Create Backlog</t>
-  </si>
-  <si>
-    <t>BurnDown</t>
-  </si>
-  <si>
-    <t>Team</t>
-  </si>
-  <si>
-    <t>Create user stories</t>
-  </si>
-  <si>
-    <t>add weekly stories to burn down chart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint Log </t>
-  </si>
-  <si>
-    <t>Log weekly sprint activities</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Work on Design Report</t>
+Release #:1.1
+Sprint #: 2</t>
+  </si>
+  <si>
+    <t>Create registration page and login page</t>
+  </si>
+  <si>
+    <t>Create Registration page</t>
+  </si>
+  <si>
+    <t>Create login page</t>
+  </si>
+  <si>
+    <t>Create Database</t>
+  </si>
+  <si>
+    <t>refactoring</t>
   </si>
 </sst>
 </file>
@@ -466,10 +457,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -894,20 +885,20 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13" style="8" customWidth="1"/>
-    <col min="3" max="3" width="21" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -982,22 +973,22 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -1015,140 +1006,74 @@
         <v>0</v>
       </c>
       <c r="L4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="7">
-        <v>2</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="7">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="7">
-        <v>4</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <v>1</v>
-      </c>
-      <c r="M7" s="4">
-        <v>1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="1"/>
@@ -1212,32 +1137,32 @@
         <v>5</v>
       </c>
       <c r="G9" s="4">
-        <f>F9 - SUM(G4:G7)</f>
+        <f t="shared" ref="G9:M9" si="1">F9 - SUM(G4:G7)</f>
         <v>5</v>
       </c>
       <c r="H9" s="4">
-        <f>G9 - SUM(H4:H7)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I9" s="4">
-        <f>H9 - SUM(I4:I7)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J9" s="4">
-        <f>I9 - SUM(J4:J7)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K9" s="4">
-        <f>J9 - SUM(K4:K7)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="L9" s="4">
-        <f>K9 - SUM(L4:L7)</f>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" si="1"/>
         <v>1</v>
-      </c>
-      <c r="M9" s="4">
-        <f>L9 - SUM(M4:M7)</f>
-        <v>0</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1829,59 +1754,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Normal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">581d4866-74cc-43f1-bef1-bb304cbfeaa5</TermId>
-        </TermInfo>
-      </Terms>
-    </DocumentBusinessValueTaxHTField0>
-    <DocumentComments xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <DocumentDepartmentTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Academic Program and Course Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">59abafec-cbf5-4238-a796-a3b74278f4db</TermId>
-        </TermInfo>
-      </Terms>
-    </DocumentDepartmentTaxHTField0>
-    <DocumentCategoryTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentCategoryTaxHTField0>
-    <DocumentTypeTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentTypeTaxHTField0>
-    <TaxKeywordTaxHTField xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <CourseVersion xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd" xsi:nil="true"/>
-    <SecurityClassificationTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">98311b30-b9e9-4d4f-9f64-0688c0d4a234</TermId>
-        </TermInfo>
-      </Terms>
-    </SecurityClassificationTaxHTField0>
-    <TaxCatchAll xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <DocumentSubjectTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentSubjectTaxHTField0>
-    <DocumentStatusTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentStatusTaxHTField0>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>False</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Course Development" ma:contentTypeID="0x010100A30BC5E90BED914E81F4B67CDEADBEEF0072B4D5296E9CCD41A4B955E8BC4A98B900B6D41DF35BCF664B888FA24C3105B583" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new Course Development document." ma:contentTypeScope="" ma:versionID="9dd9ed6e3bbe7b4f5b00c4ab3cb49488">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="30a82cfc-8d0b-455e-b705-4035c60ff9fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f302115a5f8a1b15560b600ae7cd187" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2110,48 +2006,84 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>False</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Normal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">581d4866-74cc-43f1-bef1-bb304cbfeaa5</TermId>
+        </TermInfo>
+      </Terms>
+    </DocumentBusinessValueTaxHTField0>
+    <DocumentComments xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <DocumentDepartmentTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Academic Program and Course Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">59abafec-cbf5-4238-a796-a3b74278f4db</TermId>
+        </TermInfo>
+      </Terms>
+    </DocumentDepartmentTaxHTField0>
+    <DocumentCategoryTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentCategoryTaxHTField0>
+    <DocumentTypeTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentTypeTaxHTField0>
+    <TaxKeywordTaxHTField xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <CourseVersion xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd" xsi:nil="true"/>
+    <SecurityClassificationTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">98311b30-b9e9-4d4f-9f64-0688c0d4a234</TermId>
+        </TermInfo>
+      </Terms>
+    </SecurityClassificationTaxHTField0>
+    <TaxCatchAll xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <DocumentSubjectTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentSubjectTaxHTField0>
+    <DocumentStatusTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentStatusTaxHTField0>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1ECD0D0-4518-4D57-B52A-F76CCDBAFC24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276BFEA3-D0DA-4B25-BF95-0D1383B71ED8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F2D39B0-97E8-4391-A3ED-FB030F1D954B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603F5811-AD34-4A30-8535-A7EF112BB698}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{050FE723-02E2-4B0F-87BF-0BB7B88CBE20}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2170,26 +2102,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603F5811-AD34-4A30-8535-A7EF112BB698}">
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1ECD0D0-4518-4D57-B52A-F76CCDBAFC24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F2D39B0-97E8-4391-A3ED-FB030F1D954B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276BFEA3-D0DA-4B25-BF95-0D1383B71ED8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Max progress for this week
</commit_message>
<xml_diff>
--- a/Planning and Design/Burndown Sheet.xlsx
+++ b/Planning and Design/Burndown Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\CST-247\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CB988A-B5DB-42E2-80F3-966F0F9E72E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFC374D-F687-43F9-B8F5-36352425857B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -144,27 +144,33 @@
     <t>Refactoring</t>
   </si>
   <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>Board Logic</t>
-  </si>
-  <si>
     <t>Michael</t>
   </si>
   <si>
-    <t>Button Logic</t>
-  </si>
-  <si>
-    <t>Partial Pages</t>
-  </si>
-  <si>
-    <t>Fredrick</t>
+    <t>Mark &amp; Fred</t>
+  </si>
+  <si>
+    <t>Save Game Logic</t>
+  </si>
+  <si>
+    <t>Load Game Logic</t>
+  </si>
+  <si>
+    <t>Create Save Game</t>
+  </si>
+  <si>
+    <t>Create Load Game</t>
+  </si>
+  <si>
+    <t>Research Ajax</t>
+  </si>
+  <si>
+    <t>Research Serialization</t>
   </si>
   <si>
     <t>Project Title: Minesweeper
-Release #:1.5
-Sprint #: 5</t>
+Release #:1.6
+Sprint #: 6</t>
   </si>
 </sst>
 </file>
@@ -378,33 +384,33 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down Chart'!$F$8:$M$8</c:f>
+              <c:f>'Burn Down Chart'!$F$10:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.299999999999999</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.6</c:v>
+                  <c:v>7.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8999999999999995</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1999999999999993</c:v>
+                  <c:v>4.3999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -445,30 +451,30 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down Chart'!$F$9:$M$9</c:f>
+              <c:f>'Burn Down Chart'!$F$11:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2</c:v>
@@ -593,13 +599,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>218017</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>43392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>294216</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>33867</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -893,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +915,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -996,7 +1002,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F4" s="4">
         <v>2</v>
@@ -1017,10 +1023,10 @@
         <v>0</v>
       </c>
       <c r="L4" s="4">
+        <v>2</v>
+      </c>
+      <c r="M4" s="4">
         <v>0</v>
-      </c>
-      <c r="M4" s="4">
-        <v>2</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1033,16 +1039,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -1063,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="4">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -1072,41 +1078,25 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="7">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="9" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
       <c r="L6" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M6" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1115,18 +1105,42 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="B7" s="7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="4">
+        <v>4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1.5</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="1"/>
@@ -1134,43 +1148,25 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="4">
-        <f>SUM(F4:F7)</f>
-        <v>12</v>
-      </c>
-      <c r="G8" s="4">
-        <f>ROUNDUP((F8-$F$8/7), 1)</f>
-        <v>10.299999999999999</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" ref="H8:M8" si="0">ROUNDUP((G8-$F$8/7), 1)</f>
-        <v>8.6</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="0"/>
-        <v>6.8999999999999995</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="0"/>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
       <c r="L8" s="4">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>0.5</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1179,44 +1175,18 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="4">
-        <f>SUM(F4:F7)</f>
-        <v>12</v>
-      </c>
-      <c r="G9" s="4">
-        <f t="shared" ref="G9:M9" si="1">F9 - SUM(G4:G7)</f>
-        <v>12</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="K9" s="4">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="L9" s="4">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="M9" s="4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="1"/>
@@ -1224,39 +1194,91 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="B10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="4">
+        <f>SUM(F4:F9)</f>
+        <v>10</v>
+      </c>
+      <c r="G10" s="4">
+        <f>ROUNDUP((F10-$F$10/7), 1)</f>
+        <v>8.6</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" ref="H10:M10" si="0">ROUNDUP((G10-$F$10/7), 1)</f>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="M10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+      <c r="B11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="4">
+        <f>SUM(F4:F9)</f>
+        <v>10</v>
+      </c>
+      <c r="G11" s="4">
+        <f>F11 - SUM(G4:G9)</f>
+        <v>10</v>
+      </c>
+      <c r="H11" s="4">
+        <f>G11 - SUM(H4:H9)</f>
+        <v>10</v>
+      </c>
+      <c r="I11" s="4">
+        <f>H11 - SUM(I4:I9)</f>
+        <v>10</v>
+      </c>
+      <c r="J11" s="4">
+        <f>I11 - SUM(J4:J9)</f>
+        <v>10</v>
+      </c>
+      <c r="K11" s="4">
+        <f>J11 - SUM(K4:K9)</f>
+        <v>10</v>
+      </c>
+      <c r="L11" s="4">
+        <f>K11 - SUM(L4:L9)</f>
+        <v>7</v>
+      </c>
+      <c r="M11" s="4">
+        <f>L11 - SUM(M4:M9)</f>
+        <v>2</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
@@ -1640,10 +1662,48 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1807,30 +1867,59 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Normal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">581d4866-74cc-43f1-bef1-bb304cbfeaa5</TermId>
+        </TermInfo>
+      </Terms>
+    </DocumentBusinessValueTaxHTField0>
+    <DocumentComments xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <DocumentDepartmentTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Academic Program and Course Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">59abafec-cbf5-4238-a796-a3b74278f4db</TermId>
+        </TermInfo>
+      </Terms>
+    </DocumentDepartmentTaxHTField0>
+    <DocumentCategoryTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentCategoryTaxHTField0>
+    <DocumentTypeTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentTypeTaxHTField0>
+    <TaxKeywordTaxHTField xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <CourseVersion xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd" xsi:nil="true"/>
+    <SecurityClassificationTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">98311b30-b9e9-4d4f-9f64-0688c0d4a234</TermId>
+        </TermInfo>
+      </Terms>
+    </SecurityClassificationTaxHTField0>
+    <TaxCatchAll xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <DocumentSubjectTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentSubjectTaxHTField0>
+    <DocumentStatusTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentStatusTaxHTField0>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>False</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Course Development" ma:contentTypeID="0x010100A30BC5E90BED914E81F4B67CDEADBEEF0072B4D5296E9CCD41A4B955E8BC4A98B900B6D41DF35BCF664B888FA24C3105B583" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new Course Development document." ma:contentTypeScope="" ma:versionID="9dd9ed6e3bbe7b4f5b00c4ab3cb49488">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="30a82cfc-8d0b-455e-b705-4035c60ff9fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f302115a5f8a1b15560b600ae7cd187" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2059,84 +2148,48 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>False</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Normal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">581d4866-74cc-43f1-bef1-bb304cbfeaa5</TermId>
-        </TermInfo>
-      </Terms>
-    </DocumentBusinessValueTaxHTField0>
-    <DocumentComments xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <DocumentDepartmentTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Academic Program and Course Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">59abafec-cbf5-4238-a796-a3b74278f4db</TermId>
-        </TermInfo>
-      </Terms>
-    </DocumentDepartmentTaxHTField0>
-    <DocumentCategoryTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentCategoryTaxHTField0>
-    <DocumentTypeTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentTypeTaxHTField0>
-    <TaxKeywordTaxHTField xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <CourseVersion xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd" xsi:nil="true"/>
-    <SecurityClassificationTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">98311b30-b9e9-4d4f-9f64-0688c0d4a234</TermId>
-        </TermInfo>
-      </Terms>
-    </SecurityClassificationTaxHTField0>
-    <TaxCatchAll xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <DocumentSubjectTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentSubjectTaxHTField0>
-    <DocumentStatusTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentStatusTaxHTField0>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276BFEA3-D0DA-4B25-BF95-0D1383B71ED8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1ECD0D0-4518-4D57-B52A-F76CCDBAFC24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F2D39B0-97E8-4391-A3ED-FB030F1D954B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603F5811-AD34-4A30-8535-A7EF112BB698}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{050FE723-02E2-4B0F-87BF-0BB7B88CBE20}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2155,19 +2208,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603F5811-AD34-4A30-8535-A7EF112BB698}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F2D39B0-97E8-4391-A3ED-FB030F1D954B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1ECD0D0-4518-4D57-B52A-F76CCDBAFC24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276BFEA3-D0DA-4B25-BF95-0D1383B71ED8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed Reg and Login with Partially Functioning GameBoard
</commit_message>
<xml_diff>
--- a/Planning and Design/Burndown Sheet.xlsx
+++ b/Planning and Design/Burndown Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\CST-247\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFC374D-F687-43F9-B8F5-36352425857B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F35D2E3-D1DC-4263-BB5F-A82DE71D9F35}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Task</t>
   </si>
@@ -168,9 +168,18 @@
     <t>Research Serialization</t>
   </si>
   <si>
+    <t>Fix Game Logic</t>
+  </si>
+  <si>
+    <t>Enable Flagging</t>
+  </si>
+  <si>
+    <t>Enabe Clicking</t>
+  </si>
+  <si>
     <t>Project Title: Minesweeper
-Release #:1.6
-Sprint #: 6</t>
+Release #:1.7
+Sprint #: 7</t>
   </si>
 </sst>
 </file>
@@ -384,33 +393,33 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down Chart'!$F$10:$M$10</c:f>
+              <c:f>'Burn Down Chart'!$F$11:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1999999999999993</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3999999999999995</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -451,33 +460,33 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down Chart'!$F$11:$M$11</c:f>
+              <c:f>'Burn Down Chart'!$F$12:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,13 +608,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>218017</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>43392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>294216</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>33867</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -899,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +924,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1005,7 +1014,7 @@
         <v>37</v>
       </c>
       <c r="F4" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
@@ -1023,10 +1032,10 @@
         <v>0</v>
       </c>
       <c r="L4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1175,18 +1184,42 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="B9" s="7">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+      <c r="M9" s="4">
+        <v>2</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="1"/>
@@ -1194,43 +1227,27 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F10" s="4">
-        <f>SUM(F4:F9)</f>
-        <v>10</v>
-      </c>
-      <c r="G10" s="4">
-        <f>ROUNDUP((F10-$F$10/7), 1)</f>
-        <v>8.6</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" ref="H10:M10" si="0">ROUNDUP((G10-$F$10/7), 1)</f>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="0"/>
-        <v>5.8</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="0"/>
-        <v>4.3999999999999995</v>
-      </c>
-      <c r="K10" s="4">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
       <c r="L10" s="4">
-        <f t="shared" si="0"/>
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1240,42 +1257,42 @@
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="4">
-        <f>SUM(F4:F9)</f>
-        <v>10</v>
+        <f>SUM(F4:F10)</f>
+        <v>18</v>
       </c>
       <c r="G11" s="4">
-        <f>F11 - SUM(G4:G9)</f>
-        <v>10</v>
+        <f>ROUNDUP((F11-$F$11/7), 1)</f>
+        <v>15.5</v>
       </c>
       <c r="H11" s="4">
-        <f>G11 - SUM(H4:H9)</f>
-        <v>10</v>
+        <f t="shared" ref="H11:M11" si="0">ROUNDUP((G11-$F$11/7), 1)</f>
+        <v>13</v>
       </c>
       <c r="I11" s="4">
-        <f>H11 - SUM(I4:I9)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>10.5</v>
       </c>
       <c r="J11" s="4">
-        <f>I11 - SUM(J4:J9)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="K11" s="4">
-        <f>J11 - SUM(K4:K9)</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>5.5</v>
       </c>
       <c r="L11" s="4">
-        <f>K11 - SUM(L4:L9)</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="M11" s="4">
-        <f>L11 - SUM(M4:M9)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1284,20 +1301,46 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
+      <c r="B12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="4">
+        <f>SUM(F4:F10)</f>
+        <v>18</v>
+      </c>
+      <c r="G12" s="4">
+        <f>F12 - SUM(G4:G9)</f>
+        <v>18</v>
+      </c>
+      <c r="H12" s="4">
+        <f>G12 - SUM(H4:H9)</f>
+        <v>18</v>
+      </c>
+      <c r="I12" s="4">
+        <f>H12 - SUM(I4:I9)</f>
+        <v>18</v>
+      </c>
+      <c r="J12" s="4">
+        <f>I12 - SUM(J4:J9)</f>
+        <v>18</v>
+      </c>
+      <c r="K12" s="4">
+        <f>J12 - SUM(K4:K9)</f>
+        <v>18</v>
+      </c>
+      <c r="L12" s="4">
+        <f>K12 - SUM(L4:L9)</f>
+        <v>13</v>
+      </c>
+      <c r="M12" s="4">
+        <f>L12 - SUM(M4:M9)</f>
+        <v>5</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
@@ -1700,10 +1743,29 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1867,59 +1929,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Normal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">581d4866-74cc-43f1-bef1-bb304cbfeaa5</TermId>
-        </TermInfo>
-      </Terms>
-    </DocumentBusinessValueTaxHTField0>
-    <DocumentComments xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <DocumentDepartmentTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Academic Program and Course Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">59abafec-cbf5-4238-a796-a3b74278f4db</TermId>
-        </TermInfo>
-      </Terms>
-    </DocumentDepartmentTaxHTField0>
-    <DocumentCategoryTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentCategoryTaxHTField0>
-    <DocumentTypeTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentTypeTaxHTField0>
-    <TaxKeywordTaxHTField xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <CourseVersion xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd" xsi:nil="true"/>
-    <SecurityClassificationTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">98311b30-b9e9-4d4f-9f64-0688c0d4a234</TermId>
-        </TermInfo>
-      </Terms>
-    </SecurityClassificationTaxHTField0>
-    <TaxCatchAll xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <DocumentSubjectTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentSubjectTaxHTField0>
-    <DocumentStatusTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </DocumentStatusTaxHTField0>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>False</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Course Development" ma:contentTypeID="0x010100A30BC5E90BED914E81F4B67CDEADBEEF0072B4D5296E9CCD41A4B955E8BC4A98B900B6D41DF35BCF664B888FA24C3105B583" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new Course Development document." ma:contentTypeScope="" ma:versionID="9dd9ed6e3bbe7b4f5b00c4ab3cb49488">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="30a82cfc-8d0b-455e-b705-4035c60ff9fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f302115a5f8a1b15560b600ae7cd187" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2148,48 +2181,84 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>False</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Normal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">581d4866-74cc-43f1-bef1-bb304cbfeaa5</TermId>
+        </TermInfo>
+      </Terms>
+    </DocumentBusinessValueTaxHTField0>
+    <DocumentComments xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <DocumentDepartmentTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Academic Program and Course Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">59abafec-cbf5-4238-a796-a3b74278f4db</TermId>
+        </TermInfo>
+      </Terms>
+    </DocumentDepartmentTaxHTField0>
+    <DocumentCategoryTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentCategoryTaxHTField0>
+    <DocumentTypeTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentTypeTaxHTField0>
+    <TaxKeywordTaxHTField xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <CourseVersion xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd" xsi:nil="true"/>
+    <SecurityClassificationTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">98311b30-b9e9-4d4f-9f64-0688c0d4a234</TermId>
+        </TermInfo>
+      </Terms>
+    </SecurityClassificationTaxHTField0>
+    <TaxCatchAll xmlns="30a82cfc-8d0b-455e-b705-4035c60ff9fd">
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <DocumentSubjectTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentSubjectTaxHTField0>
+    <DocumentStatusTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </DocumentStatusTaxHTField0>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1ECD0D0-4518-4D57-B52A-F76CCDBAFC24}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276BFEA3-D0DA-4B25-BF95-0D1383B71ED8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F2D39B0-97E8-4391-A3ED-FB030F1D954B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603F5811-AD34-4A30-8535-A7EF112BB698}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{050FE723-02E2-4B0F-87BF-0BB7B88CBE20}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2208,26 +2277,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603F5811-AD34-4A30-8535-A7EF112BB698}">
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1ECD0D0-4518-4D57-B52A-F76CCDBAFC24}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F2D39B0-97E8-4391-A3ED-FB030F1D954B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276BFEA3-D0DA-4B25-BF95-0D1383B71ED8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>